<commit_message>
init log in class and submit case shotrcall
</commit_message>
<xml_diff>
--- a/testCase/casedata/conferenceControl_casedate.xlsx
+++ b/testCase/casedata/conferenceControl_casedate.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>base_url</t>
   </si>
@@ -59,7 +59,13 @@
     <t>callNumber</t>
   </si>
   <si>
+    <t>9005853980</t>
+  </si>
+  <si>
     <t>device_number</t>
+  </si>
+  <si>
+    <t>20198942</t>
   </si>
 </sst>
 </file>
@@ -67,12 +73,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,12 +96,73 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -103,52 +170,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -162,33 +186,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -201,36 +230,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -241,25 +240,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -271,157 +378,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -432,6 +431,32 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -446,6 +471,33 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -479,59 +531,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -540,10 +539,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -552,144 +551,147 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1014,7 +1016,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="26.4" customHeight="1" outlineLevelCol="1"/>
@@ -1032,7 +1034,7 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1040,7 +1042,7 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1048,7 +1050,7 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1056,7 +1058,7 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1064,7 +1066,7 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1072,23 +1074,23 @@
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" ht="13.5" spans="1:2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" ht="13.5" spans="1:2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1114,13 +1116,13 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="15.875" customWidth="1"/>
-    <col min="2" max="2" width="12.775" customWidth="1"/>
+    <col min="2" max="2" width="12.775" style="1" customWidth="1"/>
     <col min="4" max="5" width="9.375"/>
     <col min="6" max="7" width="12.625"/>
   </cols>
@@ -1129,7 +1131,7 @@
       <c r="A1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1137,30 +1139,30 @@
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2">
-        <v>9005853980</v>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3">
-        <v>20734806</v>
-      </c>
-      <c r="C3">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1">
         <v>430819</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>20705276</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>20263947</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>18710881118</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>18710881116</v>
       </c>
     </row>

</xml_diff>